<commit_message>
Dark mode toggle button gigantamax
</commit_message>
<xml_diff>
--- a/todays_orders.xlsx
+++ b/todays_orders.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,152 +434,413 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>437</v>
+        <v>491</v>
       </c>
       <c r="B2" s="1">
-        <v>45725.22928240741</v>
+        <v>45733.22928240741</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="F2">
-        <v>1.3</v>
+        <v>1.8</v>
       </c>
       <c r="G2">
-        <v>1.3</v>
+        <v>1.8</v>
       </c>
       <c r="H2">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="I2" t="str">
-        <v>Butterscotch Lassi (x1), 8PM Coffee (x1)</v>
+        <v>Butterscotch Lassi (x2)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>436</v>
+        <v>490</v>
       </c>
       <c r="B3" s="1">
-        <v>45725.22928240741</v>
+        <v>45733.22928240741</v>
       </c>
       <c r="C3" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E3">
-        <v>160</v>
+        <v>1340</v>
       </c>
       <c r="F3">
-        <v>2.2</v>
+        <v>16.73</v>
       </c>
       <c r="G3">
-        <v>2.2</v>
+        <v>16.73</v>
       </c>
       <c r="H3">
-        <v>4.4</v>
+        <v>35.25</v>
       </c>
       <c r="I3" t="str">
-        <v>Butterscotch Lassi (x2), 8PM Coffee (x1)</v>
+        <v>Chicken Burger (x1), Chicken Cheese Burger (x1), Vanilla Shake (x1), Oreo Shake (x1), Mango Lassi (x1), Strawberry Lassi (x1), Butterscotch Lassi (x1), Chicken Wrap (x1), Veg Wrap (x4), Chicken Cheese Pops (x1), Veg Cheese Pops (x3), Banana Shake (x2), Black Currant Shake (x1), Strawberry Shake (x1), Chocolate Shake (x1), Hard Rock Coffee (x1), 8PM Coffee (x1), Coffee Italia (x1), Belgian Coffee (x1), Lime Juice (x1)</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>435</v>
+        <v>489</v>
       </c>
       <c r="B4" s="1">
-        <v>45725.22928240741</v>
+        <v>45733.22928240741</v>
       </c>
       <c r="C4" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>330</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I4" t="str">
-        <v>Banana Shake (x2)</v>
+        <v>Strawberry Lassi (x1), Chicken Wrap (x4), Banana Shake (x1)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>433</v>
+        <v>488</v>
       </c>
       <c r="B5" s="1">
-        <v>45725.22928240741</v>
+        <v>45733.22928240741</v>
       </c>
       <c r="C5" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>190</v>
+      </c>
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="E5">
-        <v>500</v>
-      </c>
-      <c r="F5">
-        <v>7.1</v>
-      </c>
       <c r="G5">
-        <v>7.1</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="I5" t="str">
-        <v>Chicken Burger (x1), Chicken Cheese Burger (x1), Mango Lassi (x1), Strawberry Lassi (x1), Chicken Cheese Pops (x1), Veg Cheese Pops (x3)</v>
+        <v>Strawberry Lassi (x1), Chocolate Shake (x1), Hard Rock Coffee (x1), Belgian Coffee (x1), Lime Juice (x1)</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>432</v>
+        <v>487</v>
       </c>
       <c r="B6" s="1">
-        <v>45725.22928240741</v>
+        <v>45733.22928240741</v>
       </c>
       <c r="C6" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>1.25</v>
+      </c>
+      <c r="G6">
+        <v>1.25</v>
+      </c>
+      <c r="H6">
+        <v>2.5</v>
+      </c>
+      <c r="I6" t="str">
+        <v>Oreo Shake (x2)</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>486</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45733.22928240741</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>210</v>
+      </c>
+      <c r="F7">
+        <v>1.93</v>
+      </c>
+      <c r="G7">
+        <v>1.93</v>
+      </c>
+      <c r="H7">
+        <v>5.65</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Chicken Burger (x1), Chicken Cheese Burger (x1), Vanilla Shake (x1), Oreo Shake (x1)</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>485</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45733.22928240741</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>170</v>
+      </c>
+      <c r="F8">
+        <v>2.42</v>
+      </c>
+      <c r="G8">
+        <v>2.42</v>
+      </c>
+      <c r="H8">
+        <v>4.85</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Mango Lassi (x2), Veg Wrap (x1)</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>484</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45733.22928240741</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>110</v>
+      </c>
+      <c r="F9">
+        <v>1.4</v>
+      </c>
+      <c r="G9">
+        <v>1.4</v>
+      </c>
+      <c r="H9">
+        <v>2.8</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Butterscotch Lassi (x1), Banana Shake (x1)</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>483</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45733.22928240741</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>140</v>
+      </c>
+      <c r="F10">
+        <v>2.45</v>
+      </c>
+      <c r="G10">
+        <v>2.45</v>
+      </c>
+      <c r="H10">
+        <v>4.9</v>
+      </c>
+      <c r="I10" t="str">
+        <v>Chicken Cheese Pops (x1), Veg Cheese Pops (x1)</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>482</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45733.22928240741</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>140</v>
+      </c>
+      <c r="F11">
+        <v>1.7</v>
+      </c>
+      <c r="G11">
+        <v>1.7</v>
+      </c>
+      <c r="H11">
+        <v>3.4</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Strawberry Lassi (x2), Butterscotch Lassi (x1)</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>481</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45733.22928240741</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>200</v>
+      </c>
+      <c r="F12">
         <v>4</v>
       </c>
-      <c r="E6">
-        <v>99</v>
-      </c>
-      <c r="F6">
-        <v>1.93</v>
-      </c>
-      <c r="G6">
-        <v>1.93</v>
-      </c>
-      <c r="H6">
-        <v>3.85</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Chicken Burger (x1), Strawberry Lassi (x1), Veg Wrap (x1)</v>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12" t="str">
+        <v>Banana Shake (x1), Black Currant Shake (x2), Strawberry Shake (x1)</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>480</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45733.22928240741</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>300</v>
+      </c>
+      <c r="F13">
+        <v>5.75</v>
+      </c>
+      <c r="G13">
+        <v>5.75</v>
+      </c>
+      <c r="H13">
+        <v>11.5</v>
+      </c>
+      <c r="I13" t="str">
+        <v>Chicken Cheese Burger (x1), Chicken Wrap (x2), Veg Cheese Pops (x1), Banana Shake (x1)</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>478</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45733.22928240741</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>70</v>
+      </c>
+      <c r="F14">
+        <v>1.23</v>
+      </c>
+      <c r="G14">
+        <v>1.23</v>
+      </c>
+      <c r="H14">
+        <v>2.45</v>
+      </c>
+      <c r="I14" t="str">
+        <v>Chicken Cheese Pops (x1)</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>477</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45733.22928240741</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>120</v>
+      </c>
+      <c r="F15">
+        <v>1.73</v>
+      </c>
+      <c r="G15">
+        <v>1.73</v>
+      </c>
+      <c r="H15">
+        <v>3.45</v>
+      </c>
+      <c r="I15" t="str">
+        <v>Veg Cheese Pops (x1), Banana Shake (x1)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I15"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 20px padding to a button lmao
</commit_message>
<xml_diff>
--- a/todays_orders.xlsx
+++ b/todays_orders.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,413 +434,123 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>491</v>
+        <v>578</v>
       </c>
       <c r="B2" s="1">
-        <v>45733.22928240741</v>
+        <v>45747.22928240741</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E2">
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="F2">
-        <v>1.8</v>
+        <v>3.43</v>
       </c>
       <c r="G2">
-        <v>1.8</v>
+        <v>3.43</v>
       </c>
       <c r="H2">
-        <v>3.6</v>
+        <v>6.85</v>
       </c>
       <c r="I2" t="str">
-        <v>Butterscotch Lassi (x2)</v>
+        <v>Mango Lassi (x2), Strawberry Lassi (x1), Veg Cheese Pops (x1)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>490</v>
+        <v>577</v>
       </c>
       <c r="B3" s="1">
-        <v>45733.22928240741</v>
+        <v>45747.22928240741</v>
       </c>
       <c r="C3" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D3">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>1340</v>
+        <v>150</v>
       </c>
       <c r="F3">
-        <v>16.73</v>
+        <v>1.02</v>
       </c>
       <c r="G3">
-        <v>16.73</v>
+        <v>1.02</v>
       </c>
       <c r="H3">
-        <v>35.25</v>
+        <v>3.85</v>
       </c>
       <c r="I3" t="str">
-        <v>Chicken Burger (x1), Chicken Cheese Burger (x1), Vanilla Shake (x1), Oreo Shake (x1), Mango Lassi (x1), Strawberry Lassi (x1), Butterscotch Lassi (x1), Chicken Wrap (x1), Veg Wrap (x4), Chicken Cheese Pops (x1), Veg Cheese Pops (x3), Banana Shake (x2), Black Currant Shake (x1), Strawberry Shake (x1), Chocolate Shake (x1), Hard Rock Coffee (x1), 8PM Coffee (x1), Coffee Italia (x1), Belgian Coffee (x1), Lime Juice (x1)</v>
+        <v>Chicken Cheese Burger (x1), Vanilla Shake (x1), Oreo Shake (x1)</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>489</v>
+        <v>576</v>
       </c>
       <c r="B4" s="1">
-        <v>45733.22928240741</v>
+        <v>45747.22928240741</v>
       </c>
       <c r="C4" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D4">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>330</v>
+        <v>690</v>
       </c>
       <c r="F4">
-        <v>8</v>
+        <v>10.38</v>
       </c>
       <c r="G4">
-        <v>8</v>
+        <v>10.38</v>
       </c>
       <c r="H4">
-        <v>16</v>
+        <v>20.75</v>
       </c>
       <c r="I4" t="str">
-        <v>Strawberry Lassi (x1), Chicken Wrap (x4), Banana Shake (x1)</v>
+        <v>Mango Lassi (x2), Strawberry Lassi (x3), Veg Wrap (x2), Chicken Cheese Pops (x3), Veg Cheese Pops (x2)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>488</v>
+        <v>575</v>
       </c>
       <c r="B5" s="1">
-        <v>45733.22928240741</v>
+        <v>45747.22928240741</v>
       </c>
       <c r="C5" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D5">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>190</v>
+        <v>320</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>2.6</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>2.6</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>8.8</v>
       </c>
       <c r="I5" t="str">
-        <v>Strawberry Lassi (x1), Chocolate Shake (x1), Hard Rock Coffee (x1), Belgian Coffee (x1), Lime Juice (x1)</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>487</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45733.22928240741</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D6">
-        <v>15</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="F6">
-        <v>1.25</v>
-      </c>
-      <c r="G6">
-        <v>1.25</v>
-      </c>
-      <c r="H6">
-        <v>2.5</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Oreo Shake (x2)</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>486</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45733.22928240741</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D7">
-        <v>14</v>
-      </c>
-      <c r="E7">
-        <v>210</v>
-      </c>
-      <c r="F7">
-        <v>1.93</v>
-      </c>
-      <c r="G7">
-        <v>1.93</v>
-      </c>
-      <c r="H7">
-        <v>5.65</v>
-      </c>
-      <c r="I7" t="str">
-        <v>Chicken Burger (x1), Chicken Cheese Burger (x1), Vanilla Shake (x1), Oreo Shake (x1)</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>485</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45733.22928240741</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D8">
-        <v>13</v>
-      </c>
-      <c r="E8">
-        <v>170</v>
-      </c>
-      <c r="F8">
-        <v>2.42</v>
-      </c>
-      <c r="G8">
-        <v>2.42</v>
-      </c>
-      <c r="H8">
-        <v>4.85</v>
-      </c>
-      <c r="I8" t="str">
-        <v>Mango Lassi (x2), Veg Wrap (x1)</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>484</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45733.22928240741</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-      <c r="E9">
-        <v>110</v>
-      </c>
-      <c r="F9">
-        <v>1.4</v>
-      </c>
-      <c r="G9">
-        <v>1.4</v>
-      </c>
-      <c r="H9">
-        <v>2.8</v>
-      </c>
-      <c r="I9" t="str">
-        <v>Butterscotch Lassi (x1), Banana Shake (x1)</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>483</v>
-      </c>
-      <c r="B10" s="1">
-        <v>45733.22928240741</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D10">
-        <v>11</v>
-      </c>
-      <c r="E10">
-        <v>140</v>
-      </c>
-      <c r="F10">
-        <v>2.45</v>
-      </c>
-      <c r="G10">
-        <v>2.45</v>
-      </c>
-      <c r="H10">
-        <v>4.9</v>
-      </c>
-      <c r="I10" t="str">
-        <v>Chicken Cheese Pops (x1), Veg Cheese Pops (x1)</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>482</v>
-      </c>
-      <c r="B11" s="1">
-        <v>45733.22928240741</v>
-      </c>
-      <c r="C11" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>140</v>
-      </c>
-      <c r="F11">
-        <v>1.7</v>
-      </c>
-      <c r="G11">
-        <v>1.7</v>
-      </c>
-      <c r="H11">
-        <v>3.4</v>
-      </c>
-      <c r="I11" t="str">
-        <v>Strawberry Lassi (x2), Butterscotch Lassi (x1)</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>481</v>
-      </c>
-      <c r="B12" s="1">
-        <v>45733.22928240741</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D12">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>200</v>
-      </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
-      <c r="H12">
-        <v>8</v>
-      </c>
-      <c r="I12" t="str">
-        <v>Banana Shake (x1), Black Currant Shake (x2), Strawberry Shake (x1)</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>480</v>
-      </c>
-      <c r="B13" s="1">
-        <v>45733.22928240741</v>
-      </c>
-      <c r="C13" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13">
-        <v>300</v>
-      </c>
-      <c r="F13">
-        <v>5.75</v>
-      </c>
-      <c r="G13">
-        <v>5.75</v>
-      </c>
-      <c r="H13">
-        <v>11.5</v>
-      </c>
-      <c r="I13" t="str">
-        <v>Chicken Cheese Burger (x1), Chicken Wrap (x2), Veg Cheese Pops (x1), Banana Shake (x1)</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14">
-        <v>478</v>
-      </c>
-      <c r="B14" s="1">
-        <v>45733.22928240741</v>
-      </c>
-      <c r="C14" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D14">
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <v>70</v>
-      </c>
-      <c r="F14">
-        <v>1.23</v>
-      </c>
-      <c r="G14">
-        <v>1.23</v>
-      </c>
-      <c r="H14">
-        <v>2.45</v>
-      </c>
-      <c r="I14" t="str">
-        <v>Chicken Cheese Pops (x1)</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15">
-        <v>477</v>
-      </c>
-      <c r="B15" s="1">
-        <v>45733.22928240741</v>
-      </c>
-      <c r="C15" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="E15">
-        <v>120</v>
-      </c>
-      <c r="F15">
-        <v>1.73</v>
-      </c>
-      <c r="G15">
-        <v>1.73</v>
-      </c>
-      <c r="H15">
-        <v>3.45</v>
-      </c>
-      <c r="I15" t="str">
-        <v>Veg Cheese Pops (x1), Banana Shake (x1)</v>
+        <v>Chicken Burger (x2), Chicken Cheese Burger (x2), Vanilla Shake (x2)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reduced the length of ui.js part 1 - todaysOrders has been reduced
</commit_message>
<xml_diff>
--- a/todays_orders.xlsx
+++ b/todays_orders.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,123 +434,239 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>578</v>
+        <v>593</v>
       </c>
       <c r="B2" s="1">
-        <v>45747.22928240741</v>
+        <v>45749.22928240741</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>230</v>
+        <v>60</v>
       </c>
       <c r="F2">
-        <v>3.43</v>
+        <v>0.9</v>
       </c>
       <c r="G2">
-        <v>3.43</v>
+        <v>0.9</v>
       </c>
       <c r="H2">
-        <v>6.85</v>
+        <v>1.8</v>
       </c>
       <c r="I2" t="str">
-        <v>Mango Lassi (x2), Strawberry Lassi (x1), Veg Cheese Pops (x1)</v>
+        <v>Chicken Burger (x1)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>577</v>
+        <v>592</v>
       </c>
       <c r="B3" s="1">
-        <v>45747.22928240741</v>
+        <v>45749.22928240741</v>
       </c>
       <c r="C3" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E3">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="F3">
-        <v>1.02</v>
+        <v>0.8</v>
       </c>
       <c r="G3">
-        <v>1.02</v>
+        <v>0.8</v>
       </c>
       <c r="H3">
-        <v>3.85</v>
+        <v>3.4</v>
       </c>
       <c r="I3" t="str">
-        <v>Chicken Cheese Burger (x1), Vanilla Shake (x1), Oreo Shake (x1)</v>
+        <v>Chicken Cheese Burger (x1), Vanilla Shake (x2)</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>576</v>
+        <v>591</v>
       </c>
       <c r="B4" s="1">
-        <v>45747.22928240741</v>
+        <v>45749.22928240741</v>
       </c>
       <c r="C4" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>690</v>
+        <v>80</v>
       </c>
       <c r="F4">
-        <v>10.38</v>
+        <v>0.8</v>
       </c>
       <c r="G4">
-        <v>10.38</v>
+        <v>0.8</v>
       </c>
       <c r="H4">
-        <v>20.75</v>
+        <v>1.6</v>
       </c>
       <c r="I4" t="str">
-        <v>Mango Lassi (x2), Strawberry Lassi (x3), Veg Wrap (x2), Chicken Cheese Pops (x3), Veg Cheese Pops (x2)</v>
+        <v>Belgian Coffee (x2)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>575</v>
+        <v>590</v>
       </c>
       <c r="B5" s="1">
-        <v>45747.22928240741</v>
+        <v>45749.22928240741</v>
       </c>
       <c r="C5" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>140</v>
+      </c>
+      <c r="F5">
+        <v>2.2</v>
+      </c>
+      <c r="G5">
+        <v>2.2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Belgian Coffee (x1), Lime Juice (x1), Watermelon Juice (x1), Peri Peri Fries (x2)</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>589</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45749.22928240741</v>
+      </c>
+      <c r="C6" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>220</v>
+      </c>
+      <c r="F6">
+        <v>3.1</v>
+      </c>
+      <c r="G6">
+        <v>3.1</v>
+      </c>
+      <c r="H6">
+        <v>6.2</v>
+      </c>
+      <c r="I6" t="str">
+        <v>Chicken Burger (x2), Mango Lassi (x1), Strawberry Lassi (x1)</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>588</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45749.22928240741</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>180</v>
+      </c>
+      <c r="F7">
+        <v>1.2</v>
+      </c>
+      <c r="G7">
+        <v>1.2</v>
+      </c>
+      <c r="H7">
+        <v>4.2</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Chicken Cheese Burger (x1), Vanilla Shake (x3)</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>587</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45749.22928240741</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>370</v>
+      </c>
+      <c r="F8">
+        <v>5.03</v>
+      </c>
+      <c r="G8">
+        <v>5.03</v>
+      </c>
+      <c r="H8">
+        <v>10.05</v>
+      </c>
+      <c r="I8" t="str">
+        <v>Vanilla Shake (x1), Oreo Shake (x1), Strawberry Lassi (x1), Butterscotch Lassi (x2), Chicken Wrap (x2)</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>586</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45749.22928240741</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Ajay Francis Anchan</v>
+      </c>
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>320</v>
-      </c>
-      <c r="F5">
-        <v>2.6</v>
-      </c>
-      <c r="G5">
-        <v>2.6</v>
-      </c>
-      <c r="H5">
-        <v>8.8</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Chicken Burger (x2), Chicken Cheese Burger (x2), Vanilla Shake (x2)</v>
+      <c r="E9">
+        <v>300</v>
+      </c>
+      <c r="F9">
+        <v>3.6</v>
+      </c>
+      <c r="G9">
+        <v>3.6</v>
+      </c>
+      <c r="H9">
+        <v>9</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Chicken Burger (x2), Chicken Cheese Burger (x1), Butterscotch Lassi (x2)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created the Special Statistics section
</commit_message>
<xml_diff>
--- a/todays_orders.xlsx
+++ b/todays_orders.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,239 +434,65 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>593</v>
+        <v>650</v>
       </c>
       <c r="B2" s="1">
-        <v>45749.22928240741</v>
+        <v>45761.22928240741</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>60</v>
+        <v>400</v>
       </c>
       <c r="F2">
-        <v>0.9</v>
+        <v>10</v>
       </c>
       <c r="G2">
-        <v>0.9</v>
+        <v>10</v>
       </c>
       <c r="H2">
-        <v>1.8</v>
+        <v>20</v>
       </c>
       <c r="I2" t="str">
-        <v>Chicken Burger (x1)</v>
+        <v>Strawberry Lassi (x1), Butterscotch Lassi (x6)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>592</v>
+        <v>649</v>
       </c>
       <c r="B3" s="1">
-        <v>45749.22928240741</v>
+        <v>45761.22928240741</v>
       </c>
       <c r="C3" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>140</v>
+        <v>350</v>
       </c>
       <c r="F3">
-        <v>0.8</v>
+        <v>2.3</v>
       </c>
       <c r="G3">
-        <v>0.8</v>
+        <v>2.3</v>
       </c>
       <c r="H3">
-        <v>3.4</v>
+        <v>10</v>
       </c>
       <c r="I3" t="str">
-        <v>Chicken Cheese Burger (x1), Vanilla Shake (x2)</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>591</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45749.22928240741</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>80</v>
-      </c>
-      <c r="F4">
-        <v>0.8</v>
-      </c>
-      <c r="G4">
-        <v>0.8</v>
-      </c>
-      <c r="H4">
-        <v>1.6</v>
-      </c>
-      <c r="I4" t="str">
-        <v>Belgian Coffee (x2)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>590</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45749.22928240741</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>140</v>
-      </c>
-      <c r="F5">
-        <v>2.2</v>
-      </c>
-      <c r="G5">
-        <v>2.2</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5" t="str">
-        <v>Belgian Coffee (x1), Lime Juice (x1), Watermelon Juice (x1), Peri Peri Fries (x2)</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>589</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45749.22928240741</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>220</v>
-      </c>
-      <c r="F6">
-        <v>3.1</v>
-      </c>
-      <c r="G6">
-        <v>3.1</v>
-      </c>
-      <c r="H6">
-        <v>6.2</v>
-      </c>
-      <c r="I6" t="str">
-        <v>Chicken Burger (x2), Mango Lassi (x1), Strawberry Lassi (x1)</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>588</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45749.22928240741</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>180</v>
-      </c>
-      <c r="F7">
-        <v>1.2</v>
-      </c>
-      <c r="G7">
-        <v>1.2</v>
-      </c>
-      <c r="H7">
-        <v>4.2</v>
-      </c>
-      <c r="I7" t="str">
-        <v>Chicken Cheese Burger (x1), Vanilla Shake (x3)</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>587</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45749.22928240741</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>370</v>
-      </c>
-      <c r="F8">
-        <v>5.03</v>
-      </c>
-      <c r="G8">
-        <v>5.03</v>
-      </c>
-      <c r="H8">
-        <v>10.05</v>
-      </c>
-      <c r="I8" t="str">
-        <v>Vanilla Shake (x1), Oreo Shake (x1), Strawberry Lassi (x1), Butterscotch Lassi (x2), Chicken Wrap (x2)</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>586</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45749.22928240741</v>
-      </c>
-      <c r="C9" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>300</v>
-      </c>
-      <c r="F9">
-        <v>3.6</v>
-      </c>
-      <c r="G9">
-        <v>3.6</v>
-      </c>
-      <c r="H9">
-        <v>9</v>
-      </c>
-      <c r="I9" t="str">
-        <v>Chicken Burger (x2), Chicken Cheese Burger (x1), Butterscotch Lassi (x2)</v>
+        <v>Chicken Cheese Burger (x3), Chicken Wrap (x2), Banana Shake (x1)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed unecessary left panel buttons
</commit_message>
<xml_diff>
--- a/todays_orders.xlsx
+++ b/todays_orders.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -434,65 +434,36 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>650</v>
+        <v>674</v>
       </c>
       <c r="B2" s="1">
-        <v>45761.22928240741</v>
+        <v>45763.22928240741</v>
       </c>
       <c r="C2" t="str">
         <v>Ajay Francis Anchan</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>400</v>
+        <v>580</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>14.25</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>14.25</v>
       </c>
       <c r="H2">
-        <v>20</v>
+        <v>28.5</v>
       </c>
       <c r="I2" t="str">
-        <v>Strawberry Lassi (x1), Butterscotch Lassi (x6)</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>649</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45761.22928240741</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Ajay Francis Anchan</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>350</v>
-      </c>
-      <c r="F3">
-        <v>2.3</v>
-      </c>
-      <c r="G3">
-        <v>2.3</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3" t="str">
-        <v>Chicken Cheese Burger (x3), Chicken Wrap (x2), Banana Shake (x1)</v>
+        <v>Oreo Shake (x1), Butterscotch Lassi (x4), Chicken Wrap (x4), Banana Shake (x1)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>